<commit_message>
fix percentage formatting issues in tables
</commit_message>
<xml_diff>
--- a/results_summary_tables.xlsx
+++ b/results_summary_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey\Desktop\GDES_inputs_and_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E91245F-A14F-417B-9CDF-F08E55E93C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66148813-1ECA-4F18-8FFA-7F3C627CECE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0EDC3151-48D2-41B8-B324-8D1763A7C45D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EDC3151-48D2-41B8-B324-8D1763A7C45D}"/>
   </bookViews>
   <sheets>
     <sheet name="fact_orientation_1" sheetId="1" r:id="rId1"/>
@@ -248,10 +248,10 @@
       <alignment textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -260,10 +260,10 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34115BDF-D150-450C-96A1-66771877FD51}">
   <dimension ref="A1:CO143"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BI140" sqref="BI140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,73 +597,73 @@
     <row r="1" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
       <c r="Q1" s="12"/>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
       <c r="AF1" s="12"/>
-      <c r="AG1" s="14" t="s">
+      <c r="AG1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
       <c r="AU1" s="12"/>
-      <c r="AV1" s="14" t="s">
+      <c r="AV1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="15"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="15"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
       <c r="BJ1" s="12"/>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.3">
@@ -4846,7 +4846,7 @@
       <c r="CO31" s="8"/>
     </row>
     <row r="32" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1"/>
@@ -5002,7 +5002,7 @@
       <c r="CN32" s="8"/>
     </row>
     <row r="33" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4">
         <v>0.63400000000000001</v>
@@ -5173,7 +5173,7 @@
       <c r="CO33" s="4"/>
     </row>
     <row r="34" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4">
         <v>0.58350000000000002</v>
@@ -5344,7 +5344,7 @@
       <c r="CO34" s="4"/>
     </row>
     <row r="35" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4">
         <v>0.73099999999999998</v>
@@ -5515,7 +5515,7 @@
       <c r="CO35" s="4"/>
     </row>
     <row r="36" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4">
         <v>0.45400000000000001</v>
@@ -5686,7 +5686,7 @@
       <c r="CO36" s="4"/>
     </row>
     <row r="37" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4">
         <v>0.75</v>
@@ -5857,7 +5857,7 @@
       <c r="CO37" s="4"/>
     </row>
     <row r="38" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4">
         <v>0.68500000000000005</v>
@@ -6028,7 +6028,7 @@
       <c r="CO38" s="4"/>
     </row>
     <row r="39" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4">
         <v>0.56000000000000005</v>
@@ -6199,7 +6199,7 @@
       <c r="CO39" s="4"/>
     </row>
     <row r="40" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4">
         <v>0.67849999999999999</v>
@@ -6370,7 +6370,7 @@
       <c r="CO40" s="4"/>
     </row>
     <row r="41" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4">
         <v>0.73950000000000005</v>
@@ -6541,7 +6541,7 @@
       <c r="CO41" s="4"/>
     </row>
     <row r="42" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4">
         <v>0.4425</v>
@@ -6712,7 +6712,7 @@
       <c r="CO42" s="4"/>
     </row>
     <row r="43" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
@@ -6734,7 +6734,7 @@
       <c r="CN43" s="8"/>
     </row>
     <row r="44" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1"/>
       <c r="N44" s="3">
         <v>0.7382504949035591</v>
@@ -6783,7 +6783,7 @@
       <c r="CN44" s="8"/>
     </row>
     <row r="45" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="AC45" s="3"/>
@@ -6799,7 +6799,7 @@
       <c r="CN45" s="8"/>
     </row>
     <row r="46" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1"/>
       <c r="C46" t="s">
         <v>16</v>
@@ -6947,7 +6947,7 @@
       <c r="CN46" s="8"/>
     </row>
     <row r="47" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4">
         <v>4.9742857142857137E-2</v>
@@ -7098,7 +7098,7 @@
       <c r="CO47" s="4"/>
     </row>
     <row r="48" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="1"/>
       <c r="C48" s="4">
         <v>6.6199999999999995E-2</v>
@@ -7249,7 +7249,7 @@
       <c r="CO48" s="4"/>
     </row>
     <row r="49" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1"/>
       <c r="C49" s="4">
         <v>0.10357142857142854</v>
@@ -7400,7 +7400,7 @@
       <c r="CO49" s="4"/>
     </row>
     <row r="50" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="1"/>
       <c r="C50" s="4">
         <v>0.17342857142857143</v>
@@ -7551,7 +7551,7 @@
       <c r="CO50" s="4"/>
     </row>
     <row r="51" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A51" s="19"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="1"/>
       <c r="C51" s="4">
         <v>0.12257142857142855</v>
@@ -7702,7 +7702,7 @@
       <c r="CO51" s="4"/>
     </row>
     <row r="52" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="1"/>
       <c r="C52" s="4">
         <v>6.7028571428571465E-2</v>
@@ -7853,7 +7853,7 @@
       <c r="CO52" s="4"/>
     </row>
     <row r="53" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="1"/>
       <c r="C53" s="4">
         <v>8.2814285714285688E-2</v>
@@ -8004,7 +8004,7 @@
       <c r="CO53" s="4"/>
     </row>
     <row r="54" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A54" s="19"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="1"/>
       <c r="C54" s="4">
         <v>6.3428571428571418E-2</v>
@@ -8175,7 +8175,7 @@
       <c r="CO54" s="4"/>
     </row>
     <row r="55" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="1"/>
       <c r="C55" s="4">
         <v>0.1120714285714286</v>
@@ -8346,7 +8346,7 @@
       <c r="CO55" s="4"/>
     </row>
     <row r="56" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A56" s="19"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="1"/>
       <c r="C56" s="4">
         <v>0.18492857142857141</v>
@@ -8517,7 +8517,7 @@
       <c r="CO56" s="4"/>
     </row>
     <row r="57" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1"/>
       <c r="F57">
         <v>0</v>
@@ -8847,7 +8847,7 @@
       <c r="CO59" s="8"/>
     </row>
     <row r="60" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="1"/>
@@ -9003,7 +9003,7 @@
       <c r="CN60" s="8"/>
     </row>
     <row r="61" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A61" s="19"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="1"/>
       <c r="C61" s="4">
         <v>0.41949999999999998</v>
@@ -9174,7 +9174,7 @@
       <c r="CO61" s="4"/>
     </row>
     <row r="62" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A62" s="19"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="1"/>
       <c r="C62" s="4">
         <v>0.46350000000000002</v>
@@ -9345,7 +9345,7 @@
       <c r="CO62" s="4"/>
     </row>
     <row r="63" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A63" s="19"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="1"/>
       <c r="C63" s="4">
         <v>0.48499999999999999</v>
@@ -9516,7 +9516,7 @@
       <c r="CO63" s="4"/>
     </row>
     <row r="64" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="1"/>
       <c r="C64" s="4">
         <v>0.40500000000000003</v>
@@ -9687,7 +9687,7 @@
       <c r="CO64" s="4"/>
     </row>
     <row r="65" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="1"/>
       <c r="C65" s="4">
         <v>0.41</v>
@@ -9858,7 +9858,7 @@
       <c r="CO65" s="4"/>
     </row>
     <row r="66" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="1"/>
       <c r="C66" s="4">
         <v>0.40899999999999997</v>
@@ -10029,7 +10029,7 @@
       <c r="CO66" s="4"/>
     </row>
     <row r="67" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="1"/>
       <c r="C67" s="4">
         <v>0.46474270000000001</v>
@@ -10200,7 +10200,7 @@
       <c r="CO67" s="4"/>
     </row>
     <row r="68" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="1"/>
       <c r="C68" s="4">
         <v>0.43</v>
@@ -10371,7 +10371,7 @@
       <c r="CO68" s="4"/>
     </row>
     <row r="69" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="1"/>
       <c r="C69" s="4">
         <v>0.49099999999999999</v>
@@ -10542,7 +10542,7 @@
       <c r="CO69" s="4"/>
     </row>
     <row r="70" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="1"/>
       <c r="C70" s="4">
         <v>0.4514338</v>
@@ -10713,7 +10713,7 @@
       <c r="CO70" s="4"/>
     </row>
     <row r="71" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="1"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
@@ -10738,7 +10738,7 @@
       <c r="CN71" s="8"/>
     </row>
     <row r="72" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="1"/>
       <c r="N72" s="3">
         <v>0.4699750327943007</v>
@@ -10787,7 +10787,7 @@
       <c r="CN72" s="8"/>
     </row>
     <row r="73" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="AC73" s="3"/>
@@ -10803,7 +10803,7 @@
       <c r="CN73" s="8"/>
     </row>
     <row r="74" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="1"/>
       <c r="C74" t="s">
         <v>16</v>
@@ -10951,7 +10951,7 @@
       <c r="CN74" s="8"/>
     </row>
     <row r="75" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="1"/>
       <c r="C75" s="4">
         <v>0.19268571571428569</v>
@@ -11102,7 +11102,7 @@
       <c r="CO75" s="4"/>
     </row>
     <row r="76" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="1"/>
       <c r="C76" s="4">
         <v>0.14868571571428565</v>
@@ -11253,7 +11253,7 @@
       <c r="CO76" s="4"/>
     </row>
     <row r="77" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="1"/>
       <c r="C77" s="4">
         <v>7.363571428571429E-2</v>
@@ -11404,7 +11404,7 @@
       <c r="CO77" s="4"/>
     </row>
     <row r="78" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A78" s="19"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="1"/>
       <c r="C78" s="4">
         <v>5.4707142857142843E-2</v>
@@ -11555,7 +11555,7 @@
       <c r="CO78" s="4"/>
     </row>
     <row r="79" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A79" s="19"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="1"/>
       <c r="C79" s="4">
         <v>0.20218571571428576</v>
@@ -11706,7 +11706,7 @@
       <c r="CO79" s="4"/>
     </row>
     <row r="80" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A80" s="19"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="1"/>
       <c r="C80" s="4">
         <v>0.20318571571428573</v>
@@ -11857,7 +11857,7 @@
       <c r="CO80" s="4"/>
     </row>
     <row r="81" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A81" s="19"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="1"/>
       <c r="C81" s="4">
         <v>5.236392571428572E-2</v>
@@ -12008,7 +12008,7 @@
       <c r="CO81" s="4"/>
     </row>
     <row r="82" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A82" s="19"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="1"/>
       <c r="C82" s="4">
         <v>0.18218571571428571</v>
@@ -12179,7 +12179,7 @@
       <c r="CO82" s="4"/>
     </row>
     <row r="83" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A83" s="19"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="1"/>
       <c r="C83" s="4">
         <v>0.1253428585714286</v>
@@ -12350,7 +12350,7 @@
       <c r="CO83" s="4"/>
     </row>
     <row r="84" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A84" s="19"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="1"/>
       <c r="C84" s="4">
         <v>5.5986704285714263E-2</v>
@@ -12521,7 +12521,7 @@
       <c r="CO84" s="4"/>
     </row>
     <row r="85" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A85" s="19"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="1"/>
       <c r="F85">
         <v>1</v>
@@ -12851,7 +12851,7 @@
       <c r="CO87" s="8"/>
     </row>
     <row r="88" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="1"/>
@@ -13007,7 +13007,7 @@
       <c r="CN88" s="8"/>
     </row>
     <row r="89" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A89" s="19"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="1"/>
       <c r="C89" s="4">
         <v>0.41949999999999998</v>
@@ -13176,7 +13176,7 @@
       <c r="CO89" s="4"/>
     </row>
     <row r="90" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A90" s="19"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="1"/>
       <c r="C90" s="4">
         <v>0.46350000000000002</v>
@@ -13345,7 +13345,7 @@
       <c r="CO90" s="4"/>
     </row>
     <row r="91" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A91" s="19"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="1"/>
       <c r="C91" s="4">
         <v>0.58750000000000002</v>
@@ -13498,7 +13498,7 @@
       <c r="BJ91" s="1"/>
     </row>
     <row r="92" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A92" s="19"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4">
         <v>0.5963657</v>
@@ -13651,7 +13651,7 @@
       <c r="BJ92" s="1"/>
     </row>
     <row r="93" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A93" s="19"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="1"/>
       <c r="C93" s="4">
         <v>0.41</v>
@@ -13804,7 +13804,7 @@
       <c r="BJ93" s="1"/>
     </row>
     <row r="94" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A94" s="19"/>
+      <c r="A94" s="15"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4">
         <v>0.40899999999999997</v>
@@ -13957,7 +13957,7 @@
       <c r="BJ94" s="1"/>
     </row>
     <row r="95" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A95" s="19"/>
+      <c r="A95" s="15"/>
       <c r="B95" s="1"/>
       <c r="C95" s="4">
         <v>0.7</v>
@@ -14110,7 +14110,7 @@
       <c r="BJ95" s="1"/>
     </row>
     <row r="96" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A96" s="19"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="1"/>
       <c r="C96" s="4">
         <v>0.43</v>
@@ -14263,7 +14263,7 @@
       <c r="BJ96" s="1"/>
     </row>
     <row r="97" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A97" s="19"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="1"/>
       <c r="C97" s="4">
         <v>0.49099999999999999</v>
@@ -14416,7 +14416,7 @@
       <c r="BJ97" s="1"/>
     </row>
     <row r="98" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A98" s="19"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="1"/>
       <c r="C98" s="4">
         <v>0.63581589999999999</v>
@@ -14569,7 +14569,7 @@
       <c r="BJ98" s="1"/>
     </row>
     <row r="99" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A99" s="19"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="1"/>
       <c r="Q99" s="1"/>
       <c r="AC99" s="3"/>
@@ -14586,7 +14586,7 @@
       <c r="BJ99" s="1"/>
     </row>
     <row r="100" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A100" s="19"/>
+      <c r="A100" s="15"/>
       <c r="B100" s="1"/>
       <c r="N100" s="7">
         <v>0.42917476735928817</v>
@@ -14630,7 +14630,7 @@
       <c r="BJ100" s="1"/>
     </row>
     <row r="101" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A101" s="19"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="AC101" s="3"/>
@@ -14644,7 +14644,7 @@
       <c r="BJ101" s="1"/>
     </row>
     <row r="102" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A102" s="19"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="1"/>
       <c r="C102" t="s">
         <v>16</v>
@@ -14790,7 +14790,7 @@
       <c r="BJ102" s="1"/>
     </row>
     <row r="103" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A103" s="19"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="1"/>
       <c r="C103" s="4">
         <v>0.19982857142857144</v>
@@ -14936,7 +14936,7 @@
       <c r="BJ103" s="1"/>
     </row>
     <row r="104" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A104" s="19"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="1"/>
       <c r="C104" s="4">
         <v>0.1558285714285714</v>
@@ -15082,7 +15082,7 @@
       <c r="BJ104" s="1"/>
     </row>
     <row r="105" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A105" s="19"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="1"/>
       <c r="C105" s="4">
         <v>0.1108857142857143</v>
@@ -15228,7 +15228,7 @@
       <c r="BJ105" s="1"/>
     </row>
     <row r="106" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A106" s="19"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="1"/>
       <c r="C106" s="4">
         <v>7.8985885714285706E-2</v>
@@ -15374,7 +15374,7 @@
       <c r="BJ106" s="1"/>
     </row>
     <row r="107" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A107" s="19"/>
+      <c r="A107" s="15"/>
       <c r="B107" s="1"/>
       <c r="C107" s="4">
         <v>0.20932857142857145</v>
@@ -15520,7 +15520,7 @@
       <c r="BJ107" s="1"/>
     </row>
     <row r="108" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A108" s="19"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="1"/>
       <c r="C108" s="4">
         <v>0.21032857142857148</v>
@@ -15666,7 +15666,7 @@
       <c r="BJ108" s="1"/>
     </row>
     <row r="109" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A109" s="19"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="1"/>
       <c r="C109" s="4">
         <v>0.15688571428571427</v>
@@ -15810,7 +15810,7 @@
       <c r="BJ109" s="1"/>
     </row>
     <row r="110" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A110" s="19"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="1"/>
       <c r="C110" s="4">
         <v>0.18932857142857146</v>
@@ -15976,7 +15976,7 @@
       <c r="BJ110" s="1"/>
     </row>
     <row r="111" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A111" s="19"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="1"/>
       <c r="C111" s="4">
         <v>0.12928571428571428</v>
@@ -16142,7 +16142,7 @@
       <c r="BJ111" s="1"/>
     </row>
     <row r="112" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A112" s="19"/>
+      <c r="A112" s="15"/>
       <c r="B112" s="1"/>
       <c r="C112" s="4">
         <v>9.2472694285714266E-2</v>
@@ -16308,7 +16308,7 @@
       <c r="BJ112" s="1"/>
     </row>
     <row r="113" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A113" s="19"/>
+      <c r="A113" s="15"/>
       <c r="B113" s="1"/>
       <c r="F113">
         <v>1</v>
@@ -16574,7 +16574,7 @@
       <c r="BJ115" s="1"/>
     </row>
     <row r="116" spans="1:62" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -16728,7 +16728,7 @@
       <c r="BJ116" s="1"/>
     </row>
     <row r="117" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A117" s="19"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="1"/>
       <c r="C117" s="4">
         <v>0.41949999999999998</v>
@@ -16883,7 +16883,7 @@
       <c r="BJ117" s="1"/>
     </row>
     <row r="118" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A118" s="19"/>
+      <c r="A118" s="15"/>
       <c r="B118" s="1"/>
       <c r="C118" s="4">
         <v>0.39100000000000001</v>
@@ -17038,7 +17038,7 @@
       <c r="BJ118" s="1"/>
     </row>
     <row r="119" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A119" s="19"/>
+      <c r="A119" s="15"/>
       <c r="B119" s="1"/>
       <c r="C119" s="4">
         <v>0.46</v>
@@ -17193,7 +17193,7 @@
       <c r="BJ119" s="1"/>
     </row>
     <row r="120" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A120" s="19"/>
+      <c r="A120" s="15"/>
       <c r="B120" s="1"/>
       <c r="C120" s="4">
         <v>0.38</v>
@@ -17348,7 +17348,7 @@
       <c r="BJ120" s="1"/>
     </row>
     <row r="121" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A121" s="19"/>
+      <c r="A121" s="15"/>
       <c r="B121" s="1"/>
       <c r="C121" s="4">
         <v>0.41</v>
@@ -17503,7 +17503,7 @@
       <c r="BJ121" s="1"/>
     </row>
     <row r="122" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A122" s="19"/>
+      <c r="A122" s="15"/>
       <c r="B122" s="1"/>
       <c r="C122" s="4">
         <v>0.40899999999999997</v>
@@ -17658,7 +17658,7 @@
       <c r="BJ122" s="1"/>
     </row>
     <row r="123" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A123" s="19"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="1"/>
       <c r="C123" s="4">
         <v>0.38750000000000001</v>
@@ -17813,7 +17813,7 @@
       <c r="BJ123" s="1"/>
     </row>
     <row r="124" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A124" s="19"/>
+      <c r="A124" s="15"/>
       <c r="B124" s="1"/>
       <c r="C124" s="4">
         <v>0.43</v>
@@ -17968,7 +17968,7 @@
       <c r="BJ124" s="1"/>
     </row>
     <row r="125" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A125" s="19"/>
+      <c r="A125" s="15"/>
       <c r="B125" s="1"/>
       <c r="C125" s="4">
         <v>0.4415</v>
@@ -18123,7 +18123,7 @@
       <c r="BJ125" s="1"/>
     </row>
     <row r="126" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A126" s="19"/>
+      <c r="A126" s="15"/>
       <c r="B126" s="1"/>
       <c r="C126" s="4">
         <v>0.34762670000000001</v>
@@ -18278,7 +18278,7 @@
       <c r="BJ126" s="1"/>
     </row>
     <row r="127" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A127" s="19"/>
+      <c r="A127" s="15"/>
       <c r="B127" s="1"/>
       <c r="N127" s="3"/>
       <c r="O127" s="3"/>
@@ -18295,7 +18295,7 @@
       <c r="BJ127" s="1"/>
     </row>
     <row r="128" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A128" s="19"/>
+      <c r="A128" s="15"/>
       <c r="B128" s="1"/>
       <c r="N128" s="3">
         <v>0.54335670414791015</v>
@@ -18339,7 +18339,7 @@
       <c r="BJ128" s="1"/>
     </row>
     <row r="129" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A129" s="19"/>
+      <c r="A129" s="15"/>
       <c r="B129" s="1"/>
       <c r="Q129" s="1"/>
       <c r="AC129" s="3"/>
@@ -18353,7 +18353,7 @@
       <c r="BJ129" s="1"/>
     </row>
     <row r="130" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A130" s="19"/>
+      <c r="A130" s="15"/>
       <c r="B130" s="1"/>
       <c r="C130" t="s">
         <v>16</v>
@@ -18499,7 +18499,7 @@
       <c r="BJ130" s="1"/>
     </row>
     <row r="131" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A131" s="19"/>
+      <c r="A131" s="15"/>
       <c r="B131" s="1"/>
       <c r="C131" s="4">
         <v>0.18911428571428573</v>
@@ -18645,7 +18645,7 @@
       <c r="BJ131" s="1"/>
     </row>
     <row r="132" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A132" s="19"/>
+      <c r="A132" s="15"/>
       <c r="B132" s="1"/>
       <c r="C132" s="4">
         <v>5.1207142857142875E-2</v>
@@ -18791,7 +18791,7 @@
       <c r="BJ132" s="1"/>
     </row>
     <row r="133" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A133" s="19"/>
+      <c r="A133" s="15"/>
       <c r="B133" s="1"/>
       <c r="C133" s="4">
         <v>7.3635714285714318E-2</v>
@@ -18937,7 +18937,7 @@
       <c r="BJ133" s="1"/>
     </row>
     <row r="134" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A134" s="19"/>
+      <c r="A134" s="15"/>
       <c r="B134" s="1"/>
       <c r="C134" s="4">
         <v>5.4707142857142864E-2</v>
@@ -19083,7 +19083,7 @@
       <c r="BJ134" s="1"/>
     </row>
     <row r="135" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A135" s="19"/>
+      <c r="A135" s="15"/>
       <c r="B135" s="1"/>
       <c r="C135" s="4">
         <v>0.19861428571428574</v>
@@ -19229,7 +19229,7 @@
       <c r="BJ135" s="1"/>
     </row>
     <row r="136" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A136" s="19"/>
+      <c r="A136" s="15"/>
       <c r="B136" s="1"/>
       <c r="C136" s="4">
         <v>0.19961428571428574</v>
@@ -19375,7 +19375,7 @@
       <c r="BJ136" s="1"/>
     </row>
     <row r="137" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A137" s="19"/>
+      <c r="A137" s="15"/>
       <c r="B137" s="1"/>
       <c r="C137" s="4">
         <v>5.1907142857142874E-2</v>
@@ -19521,7 +19521,7 @@
       <c r="BJ137" s="1"/>
     </row>
     <row r="138" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A138" s="19"/>
+      <c r="A138" s="15"/>
       <c r="B138" s="1"/>
       <c r="C138" s="4">
         <v>0.17861428571428573</v>
@@ -19681,13 +19681,13 @@
       <c r="BH138">
         <v>0.01</v>
       </c>
-      <c r="BI138" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI138">
+        <v>0</v>
       </c>
       <c r="BJ138" s="1"/>
     </row>
     <row r="139" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A139" s="19"/>
+      <c r="A139" s="15"/>
       <c r="B139" s="1"/>
       <c r="C139" s="4">
         <v>6.2535714285714292E-2</v>
@@ -19847,13 +19847,13 @@
       <c r="BH139">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="BI139" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI139">
+        <v>0</v>
       </c>
       <c r="BJ139" s="1"/>
     </row>
     <row r="140" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A140" s="19"/>
+      <c r="A140" s="15"/>
       <c r="B140" s="1"/>
       <c r="C140" s="4">
         <v>0.10235269571428571</v>
@@ -20019,7 +20019,7 @@
       <c r="BJ140" s="1"/>
     </row>
     <row r="141" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A141" s="19"/>
+      <c r="A141" s="15"/>
       <c r="B141" s="1"/>
       <c r="F141">
         <v>1</v>
@@ -20297,8 +20297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2031D74E-90FF-4590-BDDF-DF5675DAA65C}">
   <dimension ref="A1:CO143"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView topLeftCell="AK130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20309,73 +20309,73 @@
     <row r="1" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
       <c r="Q1" s="12"/>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
       <c r="AF1" s="12"/>
-      <c r="AG1" s="14" t="s">
+      <c r="AG1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
       <c r="AU1" s="12"/>
-      <c r="AV1" s="14" t="s">
+      <c r="AV1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="15"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="15"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
       <c r="BJ1" s="12"/>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.3">
@@ -23791,10 +23791,10 @@
         <v>2</v>
       </c>
       <c r="AC26" s="3"/>
-      <c r="AD26" s="3">
+      <c r="AD26" s="20">
         <v>0.01</v>
       </c>
-      <c r="AE26" s="3">
+      <c r="AE26" s="20">
         <v>0</v>
       </c>
       <c r="AF26" s="1"/>
@@ -23962,10 +23962,10 @@
         <v>1</v>
       </c>
       <c r="AC27" s="3"/>
-      <c r="AD27" s="3">
+      <c r="AD27" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE27" s="3">
+      <c r="AE27" s="20">
         <v>0</v>
       </c>
       <c r="AF27" s="1"/>
@@ -24133,10 +24133,10 @@
         <v>0</v>
       </c>
       <c r="AC28" s="3"/>
-      <c r="AD28" s="3">
+      <c r="AD28" s="20">
         <v>0.05</v>
       </c>
-      <c r="AE28" s="3">
+      <c r="AE28" s="20">
         <v>0</v>
       </c>
       <c r="AF28" s="1"/>
@@ -24286,10 +24286,10 @@
         <v>0.9</v>
       </c>
       <c r="AC29" s="3"/>
-      <c r="AD29" s="3">
+      <c r="AD29" s="20">
         <v>0.1</v>
       </c>
-      <c r="AE29" s="3">
+      <c r="AE29" s="20">
         <v>0</v>
       </c>
       <c r="AF29" s="1"/>
@@ -24558,7 +24558,7 @@
       <c r="CO31" s="8"/>
     </row>
     <row r="32" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1"/>
@@ -24714,7 +24714,7 @@
       <c r="CN32" s="8"/>
     </row>
     <row r="33" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4">
         <v>0.73899999999999999</v>
@@ -24885,7 +24885,7 @@
       <c r="CO33" s="4"/>
     </row>
     <row r="34" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4">
         <v>0.6825</v>
@@ -25056,7 +25056,7 @@
       <c r="CO34" s="4"/>
     </row>
     <row r="35" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4">
         <v>0.71699999999999997</v>
@@ -25227,7 +25227,7 @@
       <c r="CO35" s="4"/>
     </row>
     <row r="36" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4">
         <v>0.75</v>
@@ -25398,7 +25398,7 @@
       <c r="CO36" s="4"/>
     </row>
     <row r="37" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4">
         <v>0.70799999999999996</v>
@@ -25569,7 +25569,7 @@
       <c r="CO37" s="4"/>
     </row>
     <row r="38" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4">
         <v>0.745</v>
@@ -25740,7 +25740,7 @@
       <c r="CO38" s="4"/>
     </row>
     <row r="39" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4">
         <v>0.5</v>
@@ -25911,7 +25911,7 @@
       <c r="CO39" s="4"/>
     </row>
     <row r="40" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4">
         <v>0.70550000000000002</v>
@@ -26082,7 +26082,7 @@
       <c r="CO40" s="4"/>
     </row>
     <row r="41" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4">
         <v>0.73899999999999999</v>
@@ -26253,7 +26253,7 @@
       <c r="CO41" s="4"/>
     </row>
     <row r="42" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4">
         <v>0.72250000000000003</v>
@@ -26424,7 +26424,7 @@
       <c r="CO42" s="4"/>
     </row>
     <row r="43" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
@@ -26446,7 +26446,7 @@
       <c r="CN43" s="8"/>
     </row>
     <row r="44" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1"/>
       <c r="N44" s="3">
         <v>0.68959474649429287</v>
@@ -26495,7 +26495,7 @@
       <c r="CN44" s="8"/>
     </row>
     <row r="45" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="AC45" s="3"/>
@@ -26511,7 +26511,7 @@
       <c r="CN45" s="8"/>
     </row>
     <row r="46" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1"/>
       <c r="C46" t="s">
         <v>16</v>
@@ -26659,7 +26659,7 @@
       <c r="CN46" s="8"/>
     </row>
     <row r="47" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4">
         <v>2.9078571428571443E-2</v>
@@ -26810,7 +26810,7 @@
       <c r="CO47" s="4"/>
     </row>
     <row r="48" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="1"/>
       <c r="C48" s="4">
         <v>3.6349999999999993E-2</v>
@@ -26961,7 +26961,7 @@
       <c r="CO48" s="4"/>
     </row>
     <row r="49" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1"/>
       <c r="C49" s="4">
         <v>2.3092857142857158E-2</v>
@@ -27112,7 +27112,7 @@
       <c r="CO49" s="4"/>
     </row>
     <row r="50" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="1"/>
       <c r="C50" s="4">
         <v>3.7878571428571449E-2</v>
@@ -27263,7 +27263,7 @@
       <c r="CO50" s="4"/>
     </row>
     <row r="51" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A51" s="19"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="1"/>
       <c r="C51" s="4">
         <v>2.4892857142857161E-2</v>
@@ -27414,7 +27414,7 @@
       <c r="CO51" s="4"/>
     </row>
     <row r="52" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="1"/>
       <c r="C52" s="4">
         <v>3.3878571428571445E-2</v>
@@ -27565,7 +27565,7 @@
       <c r="CO52" s="4"/>
     </row>
     <row r="53" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="1"/>
       <c r="C53" s="4">
         <v>0.21212142857142852</v>
@@ -27716,7 +27716,7 @@
       <c r="CO53" s="4"/>
     </row>
     <row r="54" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A54" s="19"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="1"/>
       <c r="C54" s="4">
         <v>2.5392857142857151E-2</v>
@@ -27887,7 +27887,7 @@
       <c r="CO54" s="4"/>
     </row>
     <row r="55" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="1"/>
       <c r="C55" s="4">
         <v>2.9078571428571443E-2</v>
@@ -28058,7 +28058,7 @@
       <c r="CO55" s="4"/>
     </row>
     <row r="56" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A56" s="19"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="1"/>
       <c r="C56" s="4">
         <v>2.3050000000000015E-2</v>
@@ -28229,7 +28229,7 @@
       <c r="CO56" s="4"/>
     </row>
     <row r="57" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1"/>
       <c r="F57">
         <v>4</v>
@@ -28559,7 +28559,7 @@
       <c r="CO59" s="8"/>
     </row>
     <row r="60" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="1"/>
@@ -28715,7 +28715,7 @@
       <c r="CN60" s="8"/>
     </row>
     <row r="61" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A61" s="19"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="1"/>
       <c r="C61" s="4">
         <v>0.52049999999999996</v>
@@ -28886,7 +28886,7 @@
       <c r="CO61" s="4"/>
     </row>
     <row r="62" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A62" s="19"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="1"/>
       <c r="C62" s="4">
         <v>0.52300000000000002</v>
@@ -29057,7 +29057,7 @@
       <c r="CO62" s="4"/>
     </row>
     <row r="63" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A63" s="19"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="1"/>
       <c r="C63" s="4">
         <v>0.58199999999999996</v>
@@ -29228,7 +29228,7 @@
       <c r="CO63" s="4"/>
     </row>
     <row r="64" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="1"/>
       <c r="C64" s="4">
         <v>0.8</v>
@@ -29399,7 +29399,7 @@
       <c r="CO64" s="4"/>
     </row>
     <row r="65" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="1"/>
       <c r="C65" s="4">
         <v>0.51549999999999996</v>
@@ -29570,7 +29570,7 @@
       <c r="CO65" s="4"/>
     </row>
     <row r="66" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="1"/>
       <c r="C66" s="4">
         <v>0.53749999999999998</v>
@@ -29741,7 +29741,7 @@
       <c r="CO66" s="4"/>
     </row>
     <row r="67" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="1"/>
       <c r="C67" s="4">
         <v>0.6</v>
@@ -29912,7 +29912,7 @@
       <c r="CO67" s="4"/>
     </row>
     <row r="68" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="1"/>
       <c r="C68" s="4">
         <v>0.503</v>
@@ -30083,7 +30083,7 @@
       <c r="CO68" s="4"/>
     </row>
     <row r="69" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="1"/>
       <c r="C69" s="4">
         <v>0.51800000000000002</v>
@@ -30254,7 +30254,7 @@
       <c r="CO69" s="4"/>
     </row>
     <row r="70" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="1"/>
       <c r="C70" s="4">
         <v>0.68350010000000005</v>
@@ -30425,7 +30425,7 @@
       <c r="CO70" s="4"/>
     </row>
     <row r="71" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="1"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
@@ -30450,7 +30450,7 @@
       <c r="CN71" s="8"/>
     </row>
     <row r="72" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="1"/>
       <c r="N72" s="3">
         <v>0.26046643968975564</v>
@@ -30499,7 +30499,7 @@
       <c r="CN72" s="8"/>
     </row>
     <row r="73" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="AC73" s="3"/>
@@ -30515,7 +30515,7 @@
       <c r="CN73" s="8"/>
     </row>
     <row r="74" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="1"/>
       <c r="C74" t="s">
         <v>16</v>
@@ -30663,7 +30663,7 @@
       <c r="CN74" s="8"/>
     </row>
     <row r="75" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="1"/>
       <c r="C75" s="4">
         <v>6.6057148571428609E-2</v>
@@ -30814,7 +30814,7 @@
       <c r="CO75" s="4"/>
     </row>
     <row r="76" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="1"/>
       <c r="C76" s="4">
         <v>6.455714857142858E-2</v>
@@ -30965,7 +30965,7 @@
       <c r="CO76" s="4"/>
     </row>
     <row r="77" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="1"/>
       <c r="C77" s="4">
         <v>6.2371431428571399E-2</v>
@@ -31116,7 +31116,7 @@
       <c r="CO77" s="4"/>
     </row>
     <row r="78" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A78" s="19"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="1"/>
       <c r="C78" s="4">
         <v>0.22052856571428578</v>
@@ -31267,7 +31267,7 @@
       <c r="CO78" s="4"/>
     </row>
     <row r="79" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A79" s="19"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="1"/>
       <c r="C79" s="4">
         <v>6.9057148571428612E-2</v>
@@ -31418,7 +31418,7 @@
       <c r="CO79" s="4"/>
     </row>
     <row r="80" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A80" s="19"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="1"/>
       <c r="C80" s="4">
         <v>5.6971434285714315E-2</v>
@@ -31569,7 +31569,7 @@
       <c r="CO80" s="4"/>
     </row>
     <row r="81" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A81" s="19"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="1"/>
       <c r="C81" s="4">
         <v>6.9571431428571404E-2</v>
@@ -31720,7 +31720,7 @@
       <c r="CO81" s="4"/>
     </row>
     <row r="82" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A82" s="19"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="1"/>
       <c r="C82" s="4">
         <v>7.7414291428571438E-2</v>
@@ -31891,7 +31891,7 @@
       <c r="CO82" s="4"/>
     </row>
     <row r="83" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A83" s="19"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="1"/>
       <c r="C83" s="4">
         <v>6.7557148571428582E-2</v>
@@ -32062,7 +32062,7 @@
       <c r="CO83" s="4"/>
     </row>
     <row r="84" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A84" s="19"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="1"/>
       <c r="C84" s="4">
         <v>0.12732864571428576</v>
@@ -32233,7 +32233,7 @@
       <c r="CO84" s="4"/>
     </row>
     <row r="85" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A85" s="19"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="1"/>
       <c r="F85">
         <v>2</v>
@@ -32563,7 +32563,7 @@
       <c r="CO87" s="8"/>
     </row>
     <row r="88" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="1"/>
@@ -32719,7 +32719,7 @@
       <c r="CN88" s="8"/>
     </row>
     <row r="89" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A89" s="19"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="1"/>
       <c r="C89" s="4">
         <v>0.57050000000000001</v>
@@ -32888,7 +32888,7 @@
       <c r="CO89" s="4"/>
     </row>
     <row r="90" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A90" s="19"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="1"/>
       <c r="C90" s="4">
         <v>0.57299999999999995</v>
@@ -33057,7 +33057,7 @@
       <c r="CO90" s="4"/>
     </row>
     <row r="91" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A91" s="19"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="1"/>
       <c r="C91" s="4">
         <v>0.63200000000000001</v>
@@ -33210,7 +33210,7 @@
       <c r="BJ91" s="1"/>
     </row>
     <row r="92" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A92" s="19"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4">
         <v>0.85</v>
@@ -33363,7 +33363,7 @@
       <c r="BJ92" s="1"/>
     </row>
     <row r="93" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A93" s="19"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="1"/>
       <c r="C93" s="4">
         <v>0.5655</v>
@@ -33516,7 +33516,7 @@
       <c r="BJ93" s="1"/>
     </row>
     <row r="94" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A94" s="19"/>
+      <c r="A94" s="15"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4">
         <v>0.58750000000000002</v>
@@ -33669,7 +33669,7 @@
       <c r="BJ94" s="1"/>
     </row>
     <row r="95" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A95" s="19"/>
+      <c r="A95" s="15"/>
       <c r="B95" s="1"/>
       <c r="C95" s="4">
         <v>0.7</v>
@@ -33822,7 +33822,7 @@
       <c r="BJ95" s="1"/>
     </row>
     <row r="96" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A96" s="19"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="1"/>
       <c r="C96" s="4">
         <v>0.55300000000000005</v>
@@ -33975,7 +33975,7 @@
       <c r="BJ96" s="1"/>
     </row>
     <row r="97" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A97" s="19"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="1"/>
       <c r="C97" s="4">
         <v>0.56799999999999995</v>
@@ -34128,7 +34128,7 @@
       <c r="BJ97" s="1"/>
     </row>
     <row r="98" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A98" s="19"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="1"/>
       <c r="C98" s="4">
         <v>0.73350000000000004</v>
@@ -34281,7 +34281,7 @@
       <c r="BJ98" s="1"/>
     </row>
     <row r="99" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A99" s="19"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="1"/>
       <c r="Q99" s="1"/>
       <c r="AC99" s="3"/>
@@ -34298,7 +34298,7 @@
       <c r="BJ99" s="1"/>
     </row>
     <row r="100" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A100" s="19"/>
+      <c r="A100" s="15"/>
       <c r="B100" s="1"/>
       <c r="N100" s="7">
         <v>0.29559671000082693</v>
@@ -34342,7 +34342,7 @@
       <c r="BJ100" s="1"/>
     </row>
     <row r="101" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A101" s="19"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="AC101" s="3"/>
@@ -34356,7 +34356,7 @@
       <c r="BJ101" s="1"/>
     </row>
     <row r="102" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A102" s="19"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="1"/>
       <c r="C102" t="s">
         <v>16</v>
@@ -34502,7 +34502,7 @@
       <c r="BJ102" s="1"/>
     </row>
     <row r="103" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A103" s="19"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="1"/>
       <c r="C103" s="4">
         <v>6.6057142857142856E-2</v>
@@ -34648,7 +34648,7 @@
       <c r="BJ103" s="1"/>
     </row>
     <row r="104" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A104" s="19"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="1"/>
       <c r="C104" s="4">
         <v>6.4557142857142896E-2</v>
@@ -34794,7 +34794,7 @@
       <c r="BJ104" s="1"/>
     </row>
     <row r="105" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A105" s="19"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="1"/>
       <c r="C105" s="4">
         <v>6.2371428571428543E-2</v>
@@ -34940,7 +34940,7 @@
       <c r="BJ105" s="1"/>
     </row>
     <row r="106" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A106" s="19"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="1"/>
       <c r="C106" s="4">
         <v>0.22052857142857141</v>
@@ -35086,7 +35086,7 @@
       <c r="BJ106" s="1"/>
     </row>
     <row r="107" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A107" s="19"/>
+      <c r="A107" s="15"/>
       <c r="B107" s="1"/>
       <c r="C107" s="4">
         <v>6.9057142857142859E-2</v>
@@ -35232,7 +35232,7 @@
       <c r="BJ107" s="1"/>
     </row>
     <row r="108" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A108" s="19"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="1"/>
       <c r="C108" s="4">
         <v>5.6971428571428583E-2</v>
@@ -35378,7 +35378,7 @@
       <c r="BJ108" s="1"/>
     </row>
     <row r="109" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A109" s="19"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="1"/>
       <c r="C109" s="4">
         <v>0.10052857142857134</v>
@@ -35524,7 +35524,7 @@
       <c r="BJ109" s="1"/>
     </row>
     <row r="110" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A110" s="19"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="1"/>
       <c r="C110" s="4">
         <v>7.7414285714285686E-2</v>
@@ -35690,7 +35690,7 @@
       <c r="BJ110" s="1"/>
     </row>
     <row r="111" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A111" s="19"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="1"/>
       <c r="C111" s="4">
         <v>6.7557142857142899E-2</v>
@@ -35856,7 +35856,7 @@
       <c r="BJ111" s="1"/>
     </row>
     <row r="112" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A112" s="19"/>
+      <c r="A112" s="15"/>
       <c r="B112" s="1"/>
       <c r="C112" s="4">
         <v>0.1273285714285714</v>
@@ -36022,7 +36022,7 @@
       <c r="BJ112" s="1"/>
     </row>
     <row r="113" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A113" s="19"/>
+      <c r="A113" s="15"/>
       <c r="B113" s="1"/>
       <c r="F113">
         <v>2</v>
@@ -36288,7 +36288,7 @@
       <c r="BJ115" s="1"/>
     </row>
     <row r="116" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -36442,7 +36442,7 @@
       <c r="BJ116" s="1"/>
     </row>
     <row r="117" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A117" s="19"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="1"/>
       <c r="C117" s="4">
         <v>0.4955</v>
@@ -36597,7 +36597,7 @@
       <c r="BJ117" s="1"/>
     </row>
     <row r="118" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A118" s="19"/>
+      <c r="A118" s="15"/>
       <c r="B118" s="1"/>
       <c r="C118" s="4">
         <v>0.498</v>
@@ -36752,7 +36752,7 @@
       <c r="BJ118" s="1"/>
     </row>
     <row r="119" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A119" s="19"/>
+      <c r="A119" s="15"/>
       <c r="B119" s="1"/>
       <c r="C119" s="4">
         <v>0.55700000000000005</v>
@@ -36907,7 +36907,7 @@
       <c r="BJ119" s="1"/>
     </row>
     <row r="120" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A120" s="19"/>
+      <c r="A120" s="15"/>
       <c r="B120" s="1"/>
       <c r="C120" s="4">
         <v>0.77500000000000002</v>
@@ -37062,7 +37062,7 @@
       <c r="BJ120" s="1"/>
     </row>
     <row r="121" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A121" s="19"/>
+      <c r="A121" s="15"/>
       <c r="B121" s="1"/>
       <c r="C121" s="4">
         <v>0.49049999999999999</v>
@@ -37217,7 +37217,7 @@
       <c r="BJ121" s="1"/>
     </row>
     <row r="122" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A122" s="19"/>
+      <c r="A122" s="15"/>
       <c r="B122" s="1"/>
       <c r="C122" s="4">
         <v>0.51249999999999996</v>
@@ -37372,7 +37372,7 @@
       <c r="BJ122" s="1"/>
     </row>
     <row r="123" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A123" s="19"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="1"/>
       <c r="C123" s="4">
         <v>0.55000000000000004</v>
@@ -37527,7 +37527,7 @@
       <c r="BJ123" s="1"/>
     </row>
     <row r="124" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A124" s="19"/>
+      <c r="A124" s="15"/>
       <c r="B124" s="1"/>
       <c r="C124" s="4">
         <v>0.47799999999999998</v>
@@ -37682,7 +37682,7 @@
       <c r="BJ124" s="1"/>
     </row>
     <row r="125" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A125" s="19"/>
+      <c r="A125" s="15"/>
       <c r="B125" s="1"/>
       <c r="C125" s="4">
         <v>0.49299999999999999</v>
@@ -37837,7 +37837,7 @@
       <c r="BJ125" s="1"/>
     </row>
     <row r="126" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A126" s="19"/>
+      <c r="A126" s="15"/>
       <c r="B126" s="1"/>
       <c r="C126" s="4">
         <v>0.65849999999999997</v>
@@ -37992,7 +37992,7 @@
       <c r="BJ126" s="1"/>
     </row>
     <row r="127" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A127" s="19"/>
+      <c r="A127" s="15"/>
       <c r="B127" s="1"/>
       <c r="N127" s="3"/>
       <c r="O127" s="3"/>
@@ -38009,7 +38009,7 @@
       <c r="BJ127" s="1"/>
     </row>
     <row r="128" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A128" s="19"/>
+      <c r="A128" s="15"/>
       <c r="B128" s="1"/>
       <c r="N128" s="3">
         <v>0.22646237415559106</v>
@@ -38053,7 +38053,7 @@
       <c r="BJ128" s="1"/>
     </row>
     <row r="129" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A129" s="19"/>
+      <c r="A129" s="15"/>
       <c r="B129" s="1"/>
       <c r="Q129" s="1"/>
       <c r="AC129" s="3"/>
@@ -38067,7 +38067,7 @@
       <c r="BJ129" s="1"/>
     </row>
     <row r="130" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A130" s="19"/>
+      <c r="A130" s="15"/>
       <c r="B130" s="1"/>
       <c r="C130" t="s">
         <v>16</v>
@@ -38213,7 +38213,7 @@
       <c r="BJ130" s="1"/>
     </row>
     <row r="131" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A131" s="19"/>
+      <c r="A131" s="15"/>
       <c r="B131" s="1"/>
       <c r="C131" s="4">
         <v>6.6057142857142856E-2</v>
@@ -38359,7 +38359,7 @@
       <c r="BJ131" s="1"/>
     </row>
     <row r="132" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A132" s="19"/>
+      <c r="A132" s="15"/>
       <c r="B132" s="1"/>
       <c r="C132" s="4">
         <v>6.4557142857142882E-2</v>
@@ -38505,7 +38505,7 @@
       <c r="BJ132" s="1"/>
     </row>
     <row r="133" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A133" s="19"/>
+      <c r="A133" s="15"/>
       <c r="B133" s="1"/>
       <c r="C133" s="4">
         <v>6.2371428571428612E-2</v>
@@ -38651,7 +38651,7 @@
       <c r="BJ133" s="1"/>
     </row>
     <row r="134" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A134" s="19"/>
+      <c r="A134" s="15"/>
       <c r="B134" s="1"/>
       <c r="C134" s="4">
         <v>0.22052857142857149</v>
@@ -38797,7 +38797,7 @@
       <c r="BJ134" s="1"/>
     </row>
     <row r="135" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A135" s="19"/>
+      <c r="A135" s="15"/>
       <c r="B135" s="1"/>
       <c r="C135" s="4">
         <v>6.9057142857142886E-2</v>
@@ -38943,7 +38943,7 @@
       <c r="BJ135" s="1"/>
     </row>
     <row r="136" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A136" s="19"/>
+      <c r="A136" s="15"/>
       <c r="B136" s="1"/>
       <c r="C136" s="4">
         <v>5.6971428571428603E-2</v>
@@ -39089,7 +39089,7 @@
       <c r="BJ136" s="1"/>
     </row>
     <row r="137" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A137" s="19"/>
+      <c r="A137" s="15"/>
       <c r="B137" s="1"/>
       <c r="C137" s="4">
         <v>5.9571428571428608E-2</v>
@@ -39235,7 +39235,7 @@
       <c r="BJ137" s="1"/>
     </row>
     <row r="138" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A138" s="19"/>
+      <c r="A138" s="15"/>
       <c r="B138" s="1"/>
       <c r="C138" s="4">
         <v>7.7414285714285741E-2</v>
@@ -39401,7 +39401,7 @@
       <c r="BJ138" s="1"/>
     </row>
     <row r="139" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A139" s="19"/>
+      <c r="A139" s="15"/>
       <c r="B139" s="1"/>
       <c r="C139" s="4">
         <v>6.7557142857142871E-2</v>
@@ -39567,7 +39567,7 @@
       <c r="BJ139" s="1"/>
     </row>
     <row r="140" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A140" s="19"/>
+      <c r="A140" s="15"/>
       <c r="B140" s="1"/>
       <c r="C140" s="4">
         <v>0.12732857142857143</v>
@@ -39733,7 +39733,7 @@
       <c r="BJ140" s="1"/>
     </row>
     <row r="141" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A141" s="19"/>
+      <c r="A141" s="15"/>
       <c r="B141" s="1"/>
       <c r="F141">
         <v>3</v>
@@ -39992,15 +39992,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="AV1:BI1"/>
+    <mergeCell ref="A4:A29"/>
+    <mergeCell ref="A32:A57"/>
+    <mergeCell ref="A60:A85"/>
     <mergeCell ref="A88:A113"/>
     <mergeCell ref="A116:A141"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="R1:AE1"/>
     <mergeCell ref="AG1:AT1"/>
-    <mergeCell ref="AV1:BI1"/>
-    <mergeCell ref="A4:A29"/>
-    <mergeCell ref="A32:A57"/>
-    <mergeCell ref="A60:A85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40011,8 +40011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3332D93D-E75A-4AA6-A929-DF443E5387C6}">
   <dimension ref="A1:CO143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BC146" sqref="BC146"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P110" sqref="P110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40023,73 +40023,73 @@
     <row r="1" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
       <c r="Q1" s="12"/>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
       <c r="AF1" s="12"/>
-      <c r="AG1" s="14" t="s">
+      <c r="AG1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
       <c r="AU1" s="12"/>
-      <c r="AV1" s="14" t="s">
+      <c r="AV1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="15"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="15"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
       <c r="BJ1" s="12"/>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.3">
@@ -43505,10 +43505,10 @@
         <v>2</v>
       </c>
       <c r="AC26" s="3"/>
-      <c r="AD26" s="3">
+      <c r="AD26" s="20">
         <v>0.01</v>
       </c>
-      <c r="AE26" s="3">
+      <c r="AE26" s="20">
         <v>0</v>
       </c>
       <c r="AF26" s="1"/>
@@ -43676,10 +43676,10 @@
         <v>2</v>
       </c>
       <c r="AC27" s="3"/>
-      <c r="AD27" s="3">
+      <c r="AD27" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE27" s="3">
+      <c r="AE27" s="20">
         <v>0</v>
       </c>
       <c r="AF27" s="1"/>
@@ -43847,10 +43847,10 @@
         <v>0</v>
       </c>
       <c r="AC28" s="3"/>
-      <c r="AD28" s="3">
+      <c r="AD28" s="20">
         <v>0.05</v>
       </c>
-      <c r="AE28" s="3">
+      <c r="AE28" s="20">
         <v>0</v>
       </c>
       <c r="AF28" s="1"/>
@@ -44000,10 +44000,10 @@
         <v>1.9</v>
       </c>
       <c r="AC29" s="3"/>
-      <c r="AD29" s="3">
+      <c r="AD29" s="20">
         <v>0.1</v>
       </c>
-      <c r="AE29" s="3">
+      <c r="AE29" s="20">
         <v>0</v>
       </c>
       <c r="AF29" s="1"/>
@@ -44272,7 +44272,7 @@
       <c r="CO31" s="8"/>
     </row>
     <row r="32" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1"/>
@@ -44428,7 +44428,7 @@
       <c r="CN32" s="8"/>
     </row>
     <row r="33" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4">
         <v>0.71750000000000003</v>
@@ -44599,7 +44599,7 @@
       <c r="CO33" s="4"/>
     </row>
     <row r="34" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4">
         <v>0.66949999999999998</v>
@@ -44770,7 +44770,7 @@
       <c r="CO34" s="4"/>
     </row>
     <row r="35" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4">
         <v>0.71499999999999997</v>
@@ -44941,7 +44941,7 @@
       <c r="CO35" s="4"/>
     </row>
     <row r="36" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4">
         <v>0.75</v>
@@ -45112,7 +45112,7 @@
       <c r="CO36" s="4"/>
     </row>
     <row r="37" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4">
         <v>0.71650000000000003</v>
@@ -45283,7 +45283,7 @@
       <c r="CO37" s="4"/>
     </row>
     <row r="38" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4">
         <v>0.72450000000000003</v>
@@ -45454,7 +45454,7 @@
       <c r="CO38" s="4"/>
     </row>
     <row r="39" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4">
         <v>0.5</v>
@@ -45625,7 +45625,7 @@
       <c r="CO39" s="4"/>
     </row>
     <row r="40" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4">
         <v>0.73050000000000004</v>
@@ -45796,7 +45796,7 @@
       <c r="CO40" s="4"/>
     </row>
     <row r="41" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4">
         <v>0.73350000000000004</v>
@@ -45967,7 +45967,7 @@
       <c r="CO41" s="4"/>
     </row>
     <row r="42" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4">
         <v>0.70350000000000001</v>
@@ -46138,7 +46138,7 @@
       <c r="CO42" s="4"/>
     </row>
     <row r="43" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
@@ -46160,7 +46160,7 @@
       <c r="CN43" s="8"/>
     </row>
     <row r="44" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1"/>
       <c r="N44" s="3">
         <v>0.65958762560196438</v>
@@ -46209,7 +46209,7 @@
       <c r="CN44" s="8"/>
     </row>
     <row r="45" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="AC45" s="3"/>
@@ -46225,7 +46225,7 @@
       <c r="CN45" s="8"/>
     </row>
     <row r="46" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1"/>
       <c r="C46" t="s">
         <v>16</v>
@@ -46373,7 +46373,7 @@
       <c r="CN46" s="8"/>
     </row>
     <row r="47" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4">
         <v>4.2849999999999999E-2</v>
@@ -46524,7 +46524,7 @@
       <c r="CO47" s="4"/>
     </row>
     <row r="48" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="1"/>
       <c r="C48" s="4">
         <v>4.5364285714285732E-2</v>
@@ -46675,7 +46675,7 @@
       <c r="CO48" s="4"/>
     </row>
     <row r="49" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1"/>
       <c r="C49" s="4">
         <v>4.1849999999999977E-2</v>
@@ -46826,7 +46826,7 @@
       <c r="CO49" s="4"/>
     </row>
     <row r="50" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="1"/>
       <c r="C50" s="4">
         <v>6.3207142857142851E-2</v>
@@ -46977,7 +46977,7 @@
       <c r="CO50" s="4"/>
     </row>
     <row r="51" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A51" s="19"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="1"/>
       <c r="C51" s="4">
         <v>4.2450000000000002E-2</v>
@@ -47128,7 +47128,7 @@
       <c r="CO51" s="4"/>
     </row>
     <row r="52" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="1"/>
       <c r="C52" s="4">
         <v>4.6650000000000004E-2</v>
@@ -47279,7 +47279,7 @@
       <c r="CO52" s="4"/>
     </row>
     <row r="53" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="1"/>
       <c r="C53" s="4">
         <v>0.18679285714285715</v>
@@ -47430,7 +47430,7 @@
       <c r="CO53" s="4"/>
     </row>
     <row r="54" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A54" s="19"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="1"/>
       <c r="C54" s="4">
         <v>5.0250000000000003E-2</v>
@@ -47590,8 +47590,8 @@
       <c r="BH54">
         <v>0.01</v>
       </c>
-      <c r="BI54" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI54">
+        <v>0</v>
       </c>
       <c r="BJ54" s="1"/>
       <c r="BY54" s="8"/>
@@ -47601,7 +47601,7 @@
       <c r="CO54" s="4"/>
     </row>
     <row r="55" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="1"/>
       <c r="C55" s="4">
         <v>5.2050000000000006E-2</v>
@@ -47761,8 +47761,8 @@
       <c r="BH55">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="BI55" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI55">
+        <v>0</v>
       </c>
       <c r="BJ55" s="1"/>
       <c r="BY55" s="8"/>
@@ -47772,7 +47772,7 @@
       <c r="CO55" s="4"/>
     </row>
     <row r="56" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A56" s="19"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="1"/>
       <c r="C56" s="4">
         <v>3.7407142857142847E-2</v>
@@ -47932,8 +47932,8 @@
       <c r="BH56">
         <v>0.05</v>
       </c>
-      <c r="BI56" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI56">
+        <v>0</v>
       </c>
       <c r="BJ56" s="1"/>
       <c r="BY56" s="8"/>
@@ -47943,7 +47943,7 @@
       <c r="CO56" s="4"/>
     </row>
     <row r="57" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="1"/>
       <c r="F57">
         <v>2</v>
@@ -48067,8 +48067,8 @@
       <c r="BH57">
         <v>0.1</v>
       </c>
-      <c r="BI57" t="e">
-        <v>#DIV/0!</v>
+      <c r="BI57">
+        <v>0</v>
       </c>
       <c r="BJ57" s="1"/>
       <c r="BY57" s="8"/>
@@ -48273,7 +48273,7 @@
       <c r="CO59" s="8"/>
     </row>
     <row r="60" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="1"/>
@@ -48429,7 +48429,7 @@
       <c r="CN60" s="8"/>
     </row>
     <row r="61" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A61" s="19"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="1"/>
       <c r="C61" s="4">
         <v>0.499</v>
@@ -48600,7 +48600,7 @@
       <c r="CO61" s="4"/>
     </row>
     <row r="62" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A62" s="19"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="1"/>
       <c r="C62" s="4">
         <v>0.54049999999999998</v>
@@ -48771,7 +48771,7 @@
       <c r="CO62" s="4"/>
     </row>
     <row r="63" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A63" s="19"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="1"/>
       <c r="C63" s="4">
         <v>0.60550000000000004</v>
@@ -48942,7 +48942,7 @@
       <c r="CO63" s="4"/>
     </row>
     <row r="64" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="1"/>
       <c r="C64" s="4">
         <v>0.72150000000000003</v>
@@ -49113,7 +49113,7 @@
       <c r="CO64" s="4"/>
     </row>
     <row r="65" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="15"/>
       <c r="B65" s="1"/>
       <c r="C65" s="4">
         <v>0.4945</v>
@@ -49284,7 +49284,7 @@
       <c r="CO65" s="4"/>
     </row>
     <row r="66" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="1"/>
       <c r="C66" s="4">
         <v>0.47149999999999997</v>
@@ -49455,7 +49455,7 @@
       <c r="CO66" s="4"/>
     </row>
     <row r="67" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="1"/>
       <c r="C67" s="4">
         <v>0.6</v>
@@ -49626,7 +49626,7 @@
       <c r="CO67" s="4"/>
     </row>
     <row r="68" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="1"/>
       <c r="C68" s="4">
         <v>0.52700000000000002</v>
@@ -49797,7 +49797,7 @@
       <c r="CO68" s="4"/>
     </row>
     <row r="69" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="1"/>
       <c r="C69" s="4">
         <v>0.57299999999999995</v>
@@ -49968,7 +49968,7 @@
       <c r="CO69" s="4"/>
     </row>
     <row r="70" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="1"/>
       <c r="C70" s="4">
         <v>0.75349999999999995</v>
@@ -50139,7 +50139,7 @@
       <c r="CO70" s="4"/>
     </row>
     <row r="71" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="1"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
@@ -50164,7 +50164,7 @@
       <c r="CN71" s="8"/>
     </row>
     <row r="72" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="1"/>
       <c r="N72" s="3">
         <v>0.58160876844129139</v>
@@ -50213,7 +50213,7 @@
       <c r="CN72" s="8"/>
     </row>
     <row r="73" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="AC73" s="3"/>
@@ -50229,7 +50229,7 @@
       <c r="CN73" s="8"/>
     </row>
     <row r="74" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="1"/>
       <c r="C74" t="s">
         <v>16</v>
@@ -50377,7 +50377,7 @@
       <c r="CN74" s="8"/>
     </row>
     <row r="75" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="1"/>
       <c r="C75" s="4">
         <v>0.13371428857142859</v>
@@ -50528,7 +50528,7 @@
       <c r="CO75" s="4"/>
     </row>
     <row r="76" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="1"/>
       <c r="C76" s="4">
         <v>9.2600002857142885E-2</v>
@@ -50679,7 +50679,7 @@
       <c r="CO76" s="4"/>
     </row>
     <row r="77" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="1"/>
       <c r="C77" s="4">
         <v>5.6828571428571416E-2</v>
@@ -50830,7 +50830,7 @@
       <c r="CO77" s="4"/>
     </row>
     <row r="78" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A78" s="19"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="1"/>
       <c r="C78" s="4">
         <v>0.10654285714285719</v>
@@ -50981,7 +50981,7 @@
       <c r="CO78" s="4"/>
     </row>
     <row r="79" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A79" s="19"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="1"/>
       <c r="C79" s="4">
         <v>0.13821428857142859</v>
@@ -51132,7 +51132,7 @@
       <c r="CO79" s="4"/>
     </row>
     <row r="80" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A80" s="19"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="1"/>
       <c r="C80" s="4">
         <v>0.16121428857142861</v>
@@ -51283,7 +51283,7 @@
       <c r="CO80" s="4"/>
     </row>
     <row r="81" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A81" s="19"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="1"/>
       <c r="C81" s="4">
         <v>5.7414285714285716E-2</v>
@@ -51434,7 +51434,7 @@
       <c r="CO81" s="4"/>
     </row>
     <row r="82" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A82" s="19"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="1"/>
       <c r="C82" s="4">
         <v>0.10571428857142857</v>
@@ -51605,7 +51605,7 @@
       <c r="CO82" s="4"/>
     </row>
     <row r="83" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A83" s="19"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="1"/>
       <c r="C83" s="4">
         <v>6.7542860000000038E-2</v>
@@ -51776,7 +51776,7 @@
       <c r="CO83" s="4"/>
     </row>
     <row r="84" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A84" s="19"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="1"/>
       <c r="C84" s="4">
         <v>0.12898571142857138</v>
@@ -51947,7 +51947,7 @@
       <c r="CO84" s="4"/>
     </row>
     <row r="85" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A85" s="19"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="1"/>
       <c r="F85">
         <v>0</v>
@@ -52277,7 +52277,7 @@
       <c r="CO87" s="8"/>
     </row>
     <row r="88" spans="1:93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="1"/>
@@ -52433,7 +52433,7 @@
       <c r="CN88" s="8"/>
     </row>
     <row r="89" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A89" s="19"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="1"/>
       <c r="C89" s="4">
         <v>0.54900000000000004</v>
@@ -52602,7 +52602,7 @@
       <c r="CO89" s="4"/>
     </row>
     <row r="90" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A90" s="19"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="1"/>
       <c r="C90" s="4">
         <v>0.59050000000000002</v>
@@ -52771,7 +52771,7 @@
       <c r="CO90" s="4"/>
     </row>
     <row r="91" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A91" s="19"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="1"/>
       <c r="C91" s="4">
         <v>0.65549999999999997</v>
@@ -52924,7 +52924,7 @@
       <c r="BJ91" s="1"/>
     </row>
     <row r="92" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A92" s="19"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4">
         <v>0.77149999999999996</v>
@@ -53077,7 +53077,7 @@
       <c r="BJ92" s="1"/>
     </row>
     <row r="93" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A93" s="19"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="1"/>
       <c r="C93" s="4">
         <v>0.54449999999999998</v>
@@ -53230,7 +53230,7 @@
       <c r="BJ93" s="1"/>
     </row>
     <row r="94" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A94" s="19"/>
+      <c r="A94" s="15"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4">
         <v>0.52149999999999996</v>
@@ -53383,7 +53383,7 @@
       <c r="BJ94" s="1"/>
     </row>
     <row r="95" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A95" s="19"/>
+      <c r="A95" s="15"/>
       <c r="B95" s="1"/>
       <c r="C95" s="4">
         <v>0.7</v>
@@ -53536,7 +53536,7 @@
       <c r="BJ95" s="1"/>
     </row>
     <row r="96" spans="1:93" x14ac:dyDescent="0.3">
-      <c r="A96" s="19"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="1"/>
       <c r="C96" s="4">
         <v>0.57699999999999996</v>
@@ -53689,7 +53689,7 @@
       <c r="BJ96" s="1"/>
     </row>
     <row r="97" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A97" s="19"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="1"/>
       <c r="C97" s="4">
         <v>0.623</v>
@@ -53842,7 +53842,7 @@
       <c r="BJ97" s="1"/>
     </row>
     <row r="98" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A98" s="19"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="1"/>
       <c r="C98" s="4">
         <v>0.80349999999999999</v>
@@ -53995,7 +53995,7 @@
       <c r="BJ98" s="1"/>
     </row>
     <row r="99" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A99" s="19"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="1"/>
       <c r="Q99" s="1"/>
       <c r="AC99" s="3"/>
@@ -54012,7 +54012,7 @@
       <c r="BJ99" s="1"/>
     </row>
     <row r="100" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A100" s="19"/>
+      <c r="A100" s="15"/>
       <c r="B100" s="1"/>
       <c r="N100" s="7">
         <v>0.54084210272309408</v>
@@ -54056,7 +54056,7 @@
       <c r="BJ100" s="1"/>
     </row>
     <row r="101" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A101" s="19"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="AC101" s="3"/>
@@ -54070,7 +54070,7 @@
       <c r="BJ101" s="1"/>
     </row>
     <row r="102" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A102" s="19"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="1"/>
       <c r="C102" t="s">
         <v>16</v>
@@ -54216,7 +54216,7 @@
       <c r="BJ102" s="1"/>
     </row>
     <row r="103" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A103" s="19"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="1"/>
       <c r="C103" s="4">
         <v>0.14085714285714282</v>
@@ -54362,7 +54362,7 @@
       <c r="BJ103" s="1"/>
     </row>
     <row r="104" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A104" s="19"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="1"/>
       <c r="C104" s="4">
         <v>9.9357142857142838E-2</v>
@@ -54508,7 +54508,7 @@
       <c r="BJ104" s="1"/>
     </row>
     <row r="105" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A105" s="19"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="1"/>
       <c r="C105" s="4">
         <v>5.3971428571428545E-2</v>
@@ -54654,7 +54654,7 @@
       <c r="BJ105" s="1"/>
     </row>
     <row r="106" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A106" s="19"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="1"/>
       <c r="C106" s="4">
         <v>0.10082857142857141</v>
@@ -54800,7 +54800,7 @@
       <c r="BJ106" s="1"/>
     </row>
     <row r="107" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A107" s="19"/>
+      <c r="A107" s="15"/>
       <c r="B107" s="1"/>
       <c r="C107" s="4">
         <v>0.14535714285714288</v>
@@ -54946,7 +54946,7 @@
       <c r="BJ107" s="1"/>
     </row>
     <row r="108" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A108" s="19"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="1"/>
       <c r="C108" s="4">
         <v>0.1683571428571429</v>
@@ -55016,8 +55016,6 @@
         <v>7</v>
       </c>
       <c r="AC108" s="3"/>
-      <c r="AD108" s="20"/>
-      <c r="AE108" s="20"/>
       <c r="AF108" s="1"/>
       <c r="AG108" s="4">
         <v>6.0414285714285677E-2</v>
@@ -55092,7 +55090,7 @@
       <c r="BJ108" s="1"/>
     </row>
     <row r="109" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A109" s="19"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="1"/>
       <c r="C109" s="4">
         <v>6.0414285714285677E-2</v>
@@ -55162,8 +55160,6 @@
         <v>2</v>
       </c>
       <c r="AC109" s="3"/>
-      <c r="AD109" s="20"/>
-      <c r="AE109" s="20"/>
       <c r="AF109" s="1"/>
       <c r="AG109" s="4">
         <v>6.0414285714285677E-2</v>
@@ -55238,7 +55234,7 @@
       <c r="BJ109" s="1"/>
     </row>
     <row r="110" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A110" s="19"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="1"/>
       <c r="C110" s="4">
         <v>0.11285714285714291</v>
@@ -55314,10 +55310,10 @@
         <v>7</v>
       </c>
       <c r="AC110" s="3"/>
-      <c r="AD110" s="20">
+      <c r="AD110">
         <v>0.01</v>
       </c>
-      <c r="AE110" s="20">
+      <c r="AE110">
         <v>0</v>
       </c>
       <c r="AF110" s="1"/>
@@ -55404,7 +55400,7 @@
       <c r="BJ110" s="1"/>
     </row>
     <row r="111" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A111" s="19"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="1"/>
       <c r="C111" s="4">
         <v>7.231428571428572E-2</v>
@@ -55480,10 +55476,10 @@
         <v>4</v>
       </c>
       <c r="AC111" s="3"/>
-      <c r="AD111" s="20">
+      <c r="AD111">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE111" s="20">
+      <c r="AE111">
         <v>0</v>
       </c>
       <c r="AF111" s="1"/>
@@ -55570,7 +55566,7 @@
       <c r="BJ111" s="1"/>
     </row>
     <row r="112" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A112" s="19"/>
+      <c r="A112" s="15"/>
       <c r="B112" s="1"/>
       <c r="C112" s="4">
         <v>0.12184285714285711</v>
@@ -55646,10 +55642,10 @@
         <v>0</v>
       </c>
       <c r="AC112" s="3"/>
-      <c r="AD112" s="20">
+      <c r="AD112">
         <v>0.05</v>
       </c>
-      <c r="AE112" s="20">
+      <c r="AE112">
         <v>0.41666666666666669</v>
       </c>
       <c r="AF112" s="1"/>
@@ -55736,7 +55732,7 @@
       <c r="BJ112" s="1"/>
     </row>
     <row r="113" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A113" s="19"/>
+      <c r="A113" s="15"/>
       <c r="B113" s="1"/>
       <c r="F113">
         <v>2</v>
@@ -55794,10 +55790,10 @@
         <v>4.5</v>
       </c>
       <c r="AC113" s="3"/>
-      <c r="AD113" s="20">
+      <c r="AD113">
         <v>0.1</v>
       </c>
-      <c r="AE113" s="20">
+      <c r="AE113">
         <v>1.5555555555555556</v>
       </c>
       <c r="AF113" s="1"/>
@@ -56002,7 +55998,7 @@
       <c r="BJ115" s="1"/>
     </row>
     <row r="116" spans="1:62" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="1"/>
@@ -56156,7 +56152,7 @@
       <c r="BJ116" s="1"/>
     </row>
     <row r="117" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A117" s="19"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="1"/>
       <c r="C117" s="4">
         <v>0.47399999999999998</v>
@@ -56311,7 +56307,7 @@
       <c r="BJ117" s="1"/>
     </row>
     <row r="118" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A118" s="19"/>
+      <c r="A118" s="15"/>
       <c r="B118" s="1"/>
       <c r="C118" s="4">
         <v>0.51549999999999996</v>
@@ -56466,7 +56462,7 @@
       <c r="BJ118" s="1"/>
     </row>
     <row r="119" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A119" s="19"/>
+      <c r="A119" s="15"/>
       <c r="B119" s="1"/>
       <c r="C119" s="4">
         <v>0.58050000000000002</v>
@@ -56621,7 +56617,7 @@
       <c r="BJ119" s="1"/>
     </row>
     <row r="120" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A120" s="19"/>
+      <c r="A120" s="15"/>
       <c r="B120" s="1"/>
       <c r="C120" s="4">
         <v>0.69650000000000001</v>
@@ -56776,7 +56772,7 @@
       <c r="BJ120" s="1"/>
     </row>
     <row r="121" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A121" s="19"/>
+      <c r="A121" s="15"/>
       <c r="B121" s="1"/>
       <c r="C121" s="4">
         <v>0.46949999999999997</v>
@@ -56931,7 +56927,7 @@
       <c r="BJ121" s="1"/>
     </row>
     <row r="122" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A122" s="19"/>
+      <c r="A122" s="15"/>
       <c r="B122" s="1"/>
       <c r="C122" s="4">
         <v>0.44650000000000001</v>
@@ -57086,7 +57082,7 @@
       <c r="BJ122" s="1"/>
     </row>
     <row r="123" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A123" s="19"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="1"/>
       <c r="C123" s="4">
         <v>0.55000000000000004</v>
@@ -57241,7 +57237,7 @@
       <c r="BJ123" s="1"/>
     </row>
     <row r="124" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A124" s="19"/>
+      <c r="A124" s="15"/>
       <c r="B124" s="1"/>
       <c r="C124" s="4">
         <v>0.502</v>
@@ -57396,7 +57392,7 @@
       <c r="BJ124" s="1"/>
     </row>
     <row r="125" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A125" s="19"/>
+      <c r="A125" s="15"/>
       <c r="B125" s="1"/>
       <c r="C125" s="4">
         <v>0.54800000000000004</v>
@@ -57551,7 +57547,7 @@
       <c r="BJ125" s="1"/>
     </row>
     <row r="126" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A126" s="19"/>
+      <c r="A126" s="15"/>
       <c r="B126" s="1"/>
       <c r="C126" s="4">
         <v>0.72850000000000004</v>
@@ -57706,7 +57702,7 @@
       <c r="BJ126" s="1"/>
     </row>
     <row r="127" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A127" s="19"/>
+      <c r="A127" s="15"/>
       <c r="B127" s="1"/>
       <c r="N127" s="3"/>
       <c r="O127" s="3"/>
@@ -57723,7 +57719,7 @@
       <c r="BJ127" s="1"/>
     </row>
     <row r="128" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A128" s="19"/>
+      <c r="A128" s="15"/>
       <c r="B128" s="1"/>
       <c r="N128" s="3">
         <v>0.58085038026515368</v>
@@ -57767,7 +57763,7 @@
       <c r="BJ128" s="1"/>
     </row>
     <row r="129" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A129" s="19"/>
+      <c r="A129" s="15"/>
       <c r="B129" s="1"/>
       <c r="Q129" s="1"/>
       <c r="AC129" s="3"/>
@@ -57781,7 +57777,7 @@
       <c r="BJ129" s="1"/>
     </row>
     <row r="130" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A130" s="19"/>
+      <c r="A130" s="15"/>
       <c r="B130" s="1"/>
       <c r="C130" t="s">
         <v>16</v>
@@ -57927,7 +57923,7 @@
       <c r="BJ130" s="1"/>
     </row>
     <row r="131" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A131" s="19"/>
+      <c r="A131" s="15"/>
       <c r="B131" s="1"/>
       <c r="C131" s="4">
         <v>0.13014285714285714</v>
@@ -58073,7 +58069,7 @@
       <c r="BJ131" s="1"/>
     </row>
     <row r="132" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A132" s="19"/>
+      <c r="A132" s="15"/>
       <c r="B132" s="1"/>
       <c r="C132" s="4">
         <v>8.974285714285718E-2</v>
@@ -58219,7 +58215,7 @@
       <c r="BJ132" s="1"/>
     </row>
     <row r="133" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A133" s="19"/>
+      <c r="A133" s="15"/>
       <c r="B133" s="1"/>
       <c r="C133" s="4">
         <v>5.8257142857142841E-2</v>
@@ -58365,7 +58361,7 @@
       <c r="BJ133" s="1"/>
     </row>
     <row r="134" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A134" s="19"/>
+      <c r="A134" s="15"/>
       <c r="B134" s="1"/>
       <c r="C134" s="4">
         <v>0.10939999999999998</v>
@@ -58511,7 +58507,7 @@
       <c r="BJ134" s="1"/>
     </row>
     <row r="135" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A135" s="19"/>
+      <c r="A135" s="15"/>
       <c r="B135" s="1"/>
       <c r="C135" s="4">
         <v>0.13464285714285718</v>
@@ -58657,7 +58653,7 @@
       <c r="BJ135" s="1"/>
     </row>
     <row r="136" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A136" s="19"/>
+      <c r="A136" s="15"/>
       <c r="B136" s="1"/>
       <c r="C136" s="4">
         <v>0.15764285714285711</v>
@@ -58803,7 +58799,7 @@
       <c r="BJ136" s="1"/>
     </row>
     <row r="137" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A137" s="19"/>
+      <c r="A137" s="15"/>
       <c r="B137" s="1"/>
       <c r="C137" s="4">
         <v>6.7328571428571418E-2</v>
@@ -58949,7 +58945,7 @@
       <c r="BJ137" s="1"/>
     </row>
     <row r="138" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A138" s="19"/>
+      <c r="A138" s="15"/>
       <c r="B138" s="1"/>
       <c r="C138" s="4">
         <v>0.10214285714285713</v>
@@ -59115,7 +59111,7 @@
       <c r="BJ138" s="1"/>
     </row>
     <row r="139" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A139" s="19"/>
+      <c r="A139" s="15"/>
       <c r="B139" s="1"/>
       <c r="C139" s="4">
         <v>6.8128571428571413E-2</v>
@@ -59281,7 +59277,7 @@
       <c r="BJ139" s="1"/>
     </row>
     <row r="140" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A140" s="19"/>
+      <c r="A140" s="15"/>
       <c r="B140" s="1"/>
       <c r="C140" s="4">
         <v>0.1325571428571429</v>
@@ -59447,7 +59443,7 @@
       <c r="BJ140" s="1"/>
     </row>
     <row r="141" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A141" s="19"/>
+      <c r="A141" s="15"/>
       <c r="B141" s="1"/>
       <c r="F141">
         <v>0</v>
@@ -59706,15 +59702,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="AV1:BI1"/>
+    <mergeCell ref="A4:A29"/>
+    <mergeCell ref="A32:A57"/>
+    <mergeCell ref="A60:A85"/>
     <mergeCell ref="A88:A113"/>
     <mergeCell ref="A116:A141"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="R1:AE1"/>
     <mergeCell ref="AG1:AT1"/>
-    <mergeCell ref="AV1:BI1"/>
-    <mergeCell ref="A4:A29"/>
-    <mergeCell ref="A32:A57"/>
-    <mergeCell ref="A60:A85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>